<commit_message>
Example of 2D gaussian surface
</commit_message>
<xml_diff>
--- a/2DGaussKernel(5pix).xlsx
+++ b/2DGaussKernel(5pix).xlsx
@@ -4,20 +4,28 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1455" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="1905" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="2D KERNEL VALUES" sheetId="1" r:id="rId1"/>
+    <sheet name="2D KERNEL SURFACE" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>2D KERNEL SURFACE</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -25,13 +33,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,7 +76,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -54,6 +84,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -179,7 +213,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$1:$BI$1</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$1:$BI$1</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -419,7 +453,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$2:$BI$2</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$2:$BI$2</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -659,7 +693,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$3:$BI$3</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$3:$BI$3</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -899,7 +933,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$4:$BI$4</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$4:$BI$4</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -1139,7 +1173,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$5:$BI$5</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$5:$BI$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -1379,7 +1413,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$6:$BI$6</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$6:$BI$6</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -1622,7 +1656,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$7:$BI$7</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$7:$BI$7</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -1865,7 +1899,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$8:$BI$8</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$8:$BI$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -2108,7 +2142,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$9:$BI$9</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$9:$BI$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -2351,7 +2385,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$10:$BI$10</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$10:$BI$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -2594,7 +2628,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$11:$BI$11</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$11:$BI$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -2837,7 +2871,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$12:$BI$12</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$12:$BI$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -3083,7 +3117,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$13:$BI$13</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$13:$BI$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -3329,7 +3363,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$14:$BI$14</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$14:$BI$14</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -3575,7 +3609,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$15:$BI$15</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$15:$BI$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -3821,7 +3855,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$16:$BI$16</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$16:$BI$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -4067,7 +4101,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$17:$BI$17</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$17:$BI$17</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -4313,7 +4347,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$18:$BI$18</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$18:$BI$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -4556,7 +4590,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$19:$BI$19</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$19:$BI$19</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -4799,7 +4833,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$20:$BI$20</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$20:$BI$20</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -5042,7 +5076,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$21:$BI$21</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$21:$BI$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -5285,7 +5319,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$22:$BI$22</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$22:$BI$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -5528,7 +5562,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$23:$BI$23</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$23:$BI$23</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -5771,7 +5805,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$24:$BI$24</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$24:$BI$24</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -6017,7 +6051,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$25:$BI$25</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$25:$BI$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -6263,7 +6297,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$26:$BI$26</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$26:$BI$26</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -6509,7 +6543,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$27:$BI$27</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$27:$BI$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -6755,7 +6789,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$28:$BI$28</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$28:$BI$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -7001,7 +7035,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$29:$BI$29</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$29:$BI$29</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -7247,7 +7281,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$30:$BI$30</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$30:$BI$30</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -7490,7 +7524,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$31:$BI$31</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$31:$BI$31</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -7733,7 +7767,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$32:$BI$32</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$32:$BI$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -7976,7 +8010,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$33:$BI$33</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$33:$BI$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -8219,7 +8253,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$34:$BI$34</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$34:$BI$34</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -8462,7 +8496,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$35:$BI$35</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$35:$BI$35</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -8705,7 +8739,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$36:$BI$36</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$36:$BI$36</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -8951,7 +8985,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$37:$BI$37</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$37:$BI$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -9197,7 +9231,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$38:$BI$38</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$38:$BI$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -9443,7 +9477,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$39:$BI$39</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$39:$BI$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -9689,7 +9723,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$40:$BI$40</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$40:$BI$40</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -9935,7 +9969,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$41:$BI$41</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$41:$BI$41</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -10181,7 +10215,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$42:$BI$42</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$42:$BI$42</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -10424,7 +10458,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$43:$BI$43</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$43:$BI$43</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -10667,7 +10701,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$44:$BI$44</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$44:$BI$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -10910,7 +10944,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$45:$BI$45</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$45:$BI$45</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -11153,7 +11187,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$46:$BI$46</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$46:$BI$46</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -11396,7 +11430,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$47:$BI$47</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$47:$BI$47</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -11639,7 +11673,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$48:$BI$48</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$48:$BI$48</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -11885,7 +11919,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$49:$BI$49</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$49:$BI$49</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -12131,7 +12165,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$50:$BI$50</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$50:$BI$50</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -12377,7 +12411,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$51:$BI$51</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$51:$BI$51</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -12623,7 +12657,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$52:$BI$52</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$52:$BI$52</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -12869,7 +12903,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$53:$BI$53</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$53:$BI$53</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -13115,7 +13149,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$54:$BI$54</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$54:$BI$54</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -13355,7 +13389,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$55:$BI$55</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$55:$BI$55</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -13595,7 +13629,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$56:$BI$56</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$56:$BI$56</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -13835,7 +13869,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$57:$BI$57</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$57:$BI$57</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -14075,7 +14109,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$58:$BI$58</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$58:$BI$58</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -14315,7 +14349,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$59:$BI$59</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$59:$BI$59</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -14555,7 +14589,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$60:$BI$60</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$60:$BI$60</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -14798,7 +14832,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$61:$BI$61</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$61:$BI$61</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -15732,12 +15766,12 @@
             </c:spPr>
           </c:bandFmt>
         </c:bandFmts>
-        <c:axId val="-810017968"/>
-        <c:axId val="-810031024"/>
-        <c:axId val="-966958400"/>
+        <c:axId val="-676795824"/>
+        <c:axId val="-676799632"/>
+        <c:axId val="-672758368"/>
       </c:surface3DChart>
       <c:catAx>
-        <c:axId val="-810017968"/>
+        <c:axId val="-676795824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15778,7 +15812,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-810031024"/>
+        <c:crossAx val="-676799632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15786,7 +15820,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-810031024"/>
+        <c:axId val="-676799632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15836,12 +15870,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-810017968"/>
+        <c:crossAx val="-676795824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="-966958400"/>
+        <c:axId val="-672758368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15882,7 +15916,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-810031024"/>
+        <c:crossAx val="-676799632"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
       <c:spPr>
@@ -15978,7 +16012,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$1:$BI$1</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$1:$BI$1</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -16187,7 +16221,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$2:$BI$2</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$2:$BI$2</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -16396,7 +16430,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$3:$BI$3</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$3:$BI$3</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -16605,7 +16639,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$4:$BI$4</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$4:$BI$4</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -16814,7 +16848,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$5:$BI$5</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$5:$BI$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -17023,7 +17057,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$6:$BI$6</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$6:$BI$6</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -17234,7 +17268,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$7:$BI$7</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$7:$BI$7</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -17445,7 +17479,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$8:$BI$8</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$8:$BI$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -17656,7 +17690,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$9:$BI$9</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$9:$BI$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -17867,7 +17901,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$10:$BI$10</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$10:$BI$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -18078,7 +18112,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$11:$BI$11</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$11:$BI$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -18289,7 +18323,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$12:$BI$12</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$12:$BI$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -18501,7 +18535,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$13:$BI$13</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$13:$BI$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -18713,7 +18747,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$14:$BI$14</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$14:$BI$14</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -18925,7 +18959,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$15:$BI$15</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$15:$BI$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -19137,7 +19171,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$16:$BI$16</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$16:$BI$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -19349,7 +19383,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$17:$BI$17</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$17:$BI$17</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -19561,7 +19595,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$18:$BI$18</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$18:$BI$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -19772,7 +19806,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$19:$BI$19</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$19:$BI$19</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -19983,7 +20017,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$20:$BI$20</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$20:$BI$20</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -20194,7 +20228,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$21:$BI$21</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$21:$BI$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -20405,7 +20439,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$22:$BI$22</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$22:$BI$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -20616,7 +20650,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$23:$BI$23</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$23:$BI$23</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -20827,7 +20861,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$24:$BI$24</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$24:$BI$24</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -21039,7 +21073,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$25:$BI$25</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$25:$BI$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -21251,7 +21285,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$26:$BI$26</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$26:$BI$26</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -21463,7 +21497,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$27:$BI$27</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$27:$BI$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -21675,7 +21709,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$28:$BI$28</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$28:$BI$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -21887,7 +21921,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$29:$BI$29</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$29:$BI$29</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -22099,7 +22133,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$30:$BI$30</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$30:$BI$30</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -22310,7 +22344,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$31:$BI$31</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$31:$BI$31</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -22521,7 +22555,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$32:$BI$32</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$32:$BI$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -22732,7 +22766,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$33:$BI$33</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$33:$BI$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -22943,7 +22977,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$34:$BI$34</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$34:$BI$34</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -23154,7 +23188,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$35:$BI$35</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$35:$BI$35</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -23365,7 +23399,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$36:$BI$36</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$36:$BI$36</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -23577,7 +23611,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$37:$BI$37</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$37:$BI$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -23789,7 +23823,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$38:$BI$38</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$38:$BI$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -24001,7 +24035,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$39:$BI$39</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$39:$BI$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -24213,7 +24247,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$40:$BI$40</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$40:$BI$40</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -24425,7 +24459,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$41:$BI$41</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$41:$BI$41</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -24637,7 +24671,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$42:$BI$42</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$42:$BI$42</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -24848,7 +24882,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$43:$BI$43</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$43:$BI$43</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -25059,7 +25093,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$44:$BI$44</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$44:$BI$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -25270,7 +25304,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$45:$BI$45</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$45:$BI$45</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -25481,7 +25515,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$46:$BI$46</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$46:$BI$46</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -25692,7 +25726,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$47:$BI$47</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$47:$BI$47</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -25903,7 +25937,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$48:$BI$48</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$48:$BI$48</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -26115,7 +26149,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$49:$BI$49</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$49:$BI$49</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -26327,7 +26361,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$50:$BI$50</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$50:$BI$50</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -26539,7 +26573,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$51:$BI$51</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$51:$BI$51</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -26751,7 +26785,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$52:$BI$52</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$52:$BI$52</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -26963,7 +26997,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$53:$BI$53</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$53:$BI$53</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -27175,7 +27209,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$54:$BI$54</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$54:$BI$54</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -27384,7 +27418,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$55:$BI$55</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$55:$BI$55</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -27593,7 +27627,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$56:$BI$56</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$56:$BI$56</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -27802,7 +27836,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$57:$BI$57</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$57:$BI$57</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -28011,7 +28045,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$58:$BI$58</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$58:$BI$58</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -28220,7 +28254,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$59:$BI$59</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$59:$BI$59</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -28429,7 +28463,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$60:$BI$60</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$60:$BI$60</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -28640,7 +28674,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$61:$BI$61</c:f>
+              <c:f>'2D KERNEL VALUES'!$A$61:$BI$61</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -28856,11 +28890,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-612956512"/>
-        <c:axId val="-612951616"/>
+        <c:axId val="-676794736"/>
+        <c:axId val="-676794192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-612956512"/>
+        <c:axId val="-676794736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28902,7 +28936,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-612951616"/>
+        <c:crossAx val="-676794192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -28910,7 +28944,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-612951616"/>
+        <c:axId val="-676794192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28947,7 +28981,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-612956512"/>
+        <c:crossAx val="-676794736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -29591,15 +29625,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>76198</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>66673</xdr:rowOff>
+      <xdr:colOff>65252</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>44777</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>52752</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>152642</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>580260</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>142328</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -29949,13 +29983,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="AY8" sqref="AY8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AF31" sqref="AF31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="61" width="6.7109375" customWidth="1"/>
+    <col min="1" max="61" width="6.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:61" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -35599,7 +35633,7 @@
       <c r="AD31" s="2">
         <v>7.8208538795091195E-2</v>
       </c>
-      <c r="AE31" s="2">
+      <c r="AE31" s="3">
         <v>7.9788456080286493E-2</v>
       </c>
       <c r="AF31" s="2">
@@ -41269,19 +41303,30 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="I2"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="O40" sqref="O40"/>
+    <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="9" max="9" width="35.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="9:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="I2" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -41291,8 +41336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P1048576"/>
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="AB36" sqref="AB36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>